<commit_message>
working on searchbar adn the category
</commit_message>
<xml_diff>
--- a/login/User_Credentials.xlsx
+++ b/login/User_Credentials.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">testcase_number</t>
+  </si>
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -28,13 +31,25 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
+    <t xml:space="preserve">tc_001</t>
+  </si>
+  <si>
     <t xml:space="preserve">bala13012004</t>
   </si>
   <si>
     <t xml:space="preserve">balaPB@1234</t>
   </si>
   <si>
+    <t xml:space="preserve">tc_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tc_003</t>
+  </si>
+  <si>
     <t xml:space="preserve">bala13012004@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tc_004</t>
   </si>
   <si>
     <t xml:space="preserve">Bala@130105</t>
@@ -329,50 +344,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="23.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -380,9 +410,9 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="balaPB@1234"/>
-    <hyperlink ref="B4" r:id="rId2" display="balaPB@1234"/>
-    <hyperlink ref="B5" r:id="rId3" display="Bala@130105"/>
+    <hyperlink ref="C2" r:id="rId1" display="balaPB@1234"/>
+    <hyperlink ref="C4" r:id="rId2" display="balaPB@1234"/>
+    <hyperlink ref="C5" r:id="rId3" display="Bala@130105"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>